<commit_message>
On a un son maintenant
</commit_message>
<xml_diff>
--- a/Squelette_sujet_Guillaume/Squelette_sujet_Guillaume.xlsx
+++ b/Squelette_sujet_Guillaume/Squelette_sujet_Guillaume.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="36">
   <si>
     <t>Stimulus</t>
   </si>
@@ -70,6 +70,57 @@
   </si>
   <si>
     <t>melons</t>
+  </si>
+  <si>
+    <t>Une</t>
+  </si>
+  <si>
+    <t>mangue</t>
+  </si>
+  <si>
+    <t>pêche</t>
+  </si>
+  <si>
+    <t>Squelette_sujet_Guillaume_3</t>
+  </si>
+  <si>
+    <t>Squelette_sujet_Guillaume_4</t>
+  </si>
+  <si>
+    <t>Squelette_sujet_Guillaume_5</t>
+  </si>
+  <si>
+    <t>Squelette_sujet_Guillaume_6</t>
+  </si>
+  <si>
+    <t>Squelette_sujet_Guillaume_7</t>
+  </si>
+  <si>
+    <t>Un</t>
+  </si>
+  <si>
+    <t>broccolis</t>
+  </si>
+  <si>
+    <t>tomate</t>
+  </si>
+  <si>
+    <t>carottes</t>
+  </si>
+  <si>
+    <t>pêches</t>
+  </si>
+  <si>
+    <t>tomates</t>
+  </si>
+  <si>
+    <t>broccoli</t>
+  </si>
+  <si>
+    <t>carotte</t>
+  </si>
+  <si>
+    <t>e</t>
   </si>
 </sst>
 </file>
@@ -90,7 +141,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -106,11 +157,17 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -120,6 +177,12 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -129,7 +192,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H8"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="27.42578125" customWidth="true"/>
@@ -143,81 +206,211 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7" t="s">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="13" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="7" t="s">
+      <c r="C2" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2">
+        <v>4.1837613000534475</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2">
-        <v>0.36256340006366372</v>
-      </c>
-      <c r="G2" s="7" t="s">
+      <c r="E3" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3">
+        <v>2.2900279997847974</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4">
+        <v>0.43623910006135702</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5">
+        <v>0.89617410022765398</v>
+      </c>
+      <c r="G5" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="H2" t="b">
+      <c r="H5" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="7" t="s">
+    <row r="6">
+      <c r="A6" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="7" t="s">
+      <c r="C6" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6">
+        <v>1.9590281001292169</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7">
+        <v>1.5509331999346614</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3">
-        <v>0.08400959987193346</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" t="b">
-        <v>1</v>
+      <c r="E8" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8">
+        <v>0.25998409977182746</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="H8" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>